<commit_message>
Fix hlm generation (#36)
* move nb_logments to lot

* ajout du numero du lot

* manage references cadastrales

* manage references cadastrales

* remove BALCON annexe

* remove BALCON annexe

* CDC should be Caisse des dépôts et des consignations in the xlsx file

* add logements by type in doc

* add logements by type in doc
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D1C1D1-B511-FC48-BD28-6F0FD264B5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF6020E-1AAB-5E45-BC33-604CA372B835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="3060" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Loyer maxinum en €</t>
-  </si>
-  <si>
-    <t>Balcon</t>
   </si>
   <si>
     <t>Cave</t>
@@ -706,7 +703,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>17</v>
@@ -1145,7 +1142,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{591959C4-D322-A34E-A688-5466D50E7029}">
           <x14:formula1>
-            <xm:f>Data!$C$2:$C$5</xm:f>
+            <xm:f>Data!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A50</xm:sqref>
         </x14:dataValidation>
@@ -1219,9 +1216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1250,7 +1245,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1258,16 +1253,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
@@ -1278,7 +1270,7 @@
       <c r="A7" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ez/rV3sAljdu5CTfykdW72KBS67f0WLJwXD/CuUQYvGwcXcYHwcAXNQpttaoS1D20RqPqxlKDIRYREYbps4Prg==" saltValue="ax3e65c2V0k8IUCb2a0cXA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="bEDsmZ+FmACxfQF3cyUOSJYoXOIBznWdnbSx58q83o6nuQPdrWaTLPZmrKMmJTYHKXKDIN6rWdwcpkydvTos3g==" saltValue="rbBlCCMuso1zkkmD54Zvwg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix typo maxinum to maximum
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF2B7F7-F9F3-444C-BB79-5F173EBFBA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678FD94A-C49E-0046-B0B7-73FDA6CFFF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="3060" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Loyer unitaire en €</t>
   </si>
   <si>
-    <t>Loyer maxinum en €</t>
-  </si>
-  <si>
     <t>Cave</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>5. Vérifier le contenu téléversé dans l'application et enregistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
+  </si>
+  <si>
+    <t>Loyer maximum en €</t>
   </si>
 </sst>
 </file>
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1173,7 +1173,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1188,7 +1188,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
@@ -1227,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1235,7 +1235,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1243,7 +1243,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update: model logement EDD + programme begininng at row 4 for the data to upload
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -22,90 +22,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Type d'annexe exclue du calcul de la surface utile
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Choisir dans la liste déroulante. 
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">Type d'annexe exclue du calcul de la surface utile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Désignation des logements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typologie des logements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface de l'annexe en m²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loyer unitaire en €</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loyer maximum en €</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Choisir dans la liste déroulante. 
 Les annexes concernées sont ici les jardins, les caves et les surfaces de terrasse au-delà de 9 m²
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Désignation des logements
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Utilisez votre propre nomenclature, elle doit correspondre à celle indiquée dans l’EDD simplifié et dans le tableau des logements  (ex : 604, Bâtiment B, étage 4, escalier 3, logement N°604).)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Typologie des logements
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Choisir dans la liste déroulante)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface de l'annexe en m²</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loyer unitaire en €</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loyer maximum en €</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Utilisez votre propre nomenclature, elle doit correspondre à celle indiquée dans l’EDD simplifié et dans le tableau des logements  (ex : 604, Bâtiment B, étage 4, escalier 3, logement N°604).)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Choisir dans la liste déroulante)</t>
   </si>
   <si>
     <t xml:space="preserve">Ici quelques explications</t>
@@ -366,7 +312,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -380,6 +326,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -568,22 +526,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O50"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="110.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,429 +561,443 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
+    <row r="2" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="75.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="14"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="17"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+    </row>
+    <row r="7" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="20"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="8"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="13"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="13"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="8"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="16"/>
     </row>
     <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="13"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="8"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="16"/>
     </row>
     <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="13"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="11"/>
     </row>
     <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="8"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="16"/>
     </row>
     <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="13"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="11"/>
     </row>
     <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="8"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="16"/>
     </row>
     <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="13"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="11"/>
     </row>
     <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="16"/>
     </row>
     <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="18"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="22"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="11"/>
+    </row>
+    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3:C50" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C51" type="list">
       <formula1>Data!$A$2:$A$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A50" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A51" type="list">
       <formula1>Data!$C$2:$C$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1051,45 +1023,45 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="67"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="23" t="s">
-        <v>6</v>
+      <c r="B2" s="26" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1115,56 +1087,56 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>14</v>
+      <c r="A1" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>16</v>
+      <c r="A2" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>18</v>
+      <c r="A3" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>20</v>
+      <c r="A4" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="28" t="s">
-        <v>21</v>
+      <c r="A5" s="31" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
-        <v>22</v>
+      <c r="A6" s="30" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30"/>
+      <c r="A7" s="33"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="bEDsmZ+FmACxfQF3cyUOSJYoXOIBznWdnbSx58q83o6nuQPdrWaTLPZmrKMmJTYHKXKDIN6rWdwcpkydvTos3g==" saltValue="rbBlCCMuso1zkkmD54Zvwg==" spinCount="100000" sheet="true" objects="true" scenarios="true"/>

</xml_diff>

<commit_message>
S407 aide saisie fichiers xlsx (#185)
* update: xlsx files with help text

* update: model logement EDD + programme begininng at row 4 for the data to upload

* update: add "Numéro de lot des logements" in edd_files instead of type

* update: files with office + add migrations on financement and stationnement

* fix:retro-compatibility

* fix: document convention + numero lot not required
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680ECF43-F5A3-5E45-8D38-BF4E2EC1F26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CC3C32-C9B5-4672-8850-41B639590914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -102,6 +102,43 @@
   </si>
   <si>
     <t>Loyer maximum en €</t>
+  </si>
+  <si>
+    <t>(Utilisez votre propre nomenclature, elle doit correspondre à celle indiquée dans l’EDD simplifié et dans le tableau des logements  (ex : 604, Bâtiment B, étage 4, escalier 3, logement N°604).)</t>
+  </si>
+  <si>
+    <t>(Choisir dans la liste déroulante)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">exclue du calcul de la surface utile
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Choisir dans la liste déroulante. 
+Les annexes concernées sont ici les jardins, les caves et les surfaces de terrasse au-delà de 9 m²
+( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
+La déclaration des stationnements par type se fera à la prochaine étape)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -111,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +179,13 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -317,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -349,13 +393,25 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -382,7 +438,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -681,43 +737,50 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="44.75" customWidth="1"/>
+    <col min="2" max="6" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="29"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="159" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="35"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -725,7 +788,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
@@ -733,7 +796,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="20"/>
     </row>
-    <row r="5" spans="1:15" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -749,7 +812,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
@@ -765,7 +828,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -773,7 +836,7 @@
       <c r="E7" s="17"/>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
@@ -781,7 +844,7 @@
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
@@ -789,7 +852,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
@@ -797,7 +860,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -805,7 +868,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
@@ -813,7 +876,7 @@
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -821,7 +884,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
@@ -829,7 +892,7 @@
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -837,7 +900,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="18"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -845,7 +908,7 @@
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -853,7 +916,7 @@
       <c r="E17" s="17"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -861,7 +924,7 @@
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -869,7 +932,7 @@
       <c r="E19" s="17"/>
       <c r="F19" s="18"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -877,7 +940,7 @@
       <c r="E20" s="19"/>
       <c r="F20" s="20"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
@@ -885,7 +948,7 @@
       <c r="E21" s="17"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
@@ -893,7 +956,7 @@
       <c r="E22" s="19"/>
       <c r="F22" s="20"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -901,7 +964,7 @@
       <c r="E23" s="17"/>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -909,7 +972,7 @@
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -917,7 +980,7 @@
       <c r="E25" s="17"/>
       <c r="F25" s="18"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
@@ -925,7 +988,7 @@
       <c r="E26" s="19"/>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -933,7 +996,7 @@
       <c r="E27" s="17"/>
       <c r="F27" s="18"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
@@ -941,7 +1004,7 @@
       <c r="E28" s="19"/>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
@@ -949,7 +1012,7 @@
       <c r="E29" s="17"/>
       <c r="F29" s="18"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -957,7 +1020,7 @@
       <c r="E30" s="19"/>
       <c r="F30" s="20"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -965,7 +1028,7 @@
       <c r="E31" s="17"/>
       <c r="F31" s="18"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
@@ -973,7 +1036,7 @@
       <c r="E32" s="19"/>
       <c r="F32" s="20"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
@@ -981,7 +1044,7 @@
       <c r="E33" s="17"/>
       <c r="F33" s="18"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
@@ -989,7 +1052,7 @@
       <c r="E34" s="19"/>
       <c r="F34" s="20"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
@@ -997,7 +1060,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="18"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="9"/>
       <c r="C36" s="10"/>
@@ -1005,7 +1068,7 @@
       <c r="E36" s="19"/>
       <c r="F36" s="20"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
@@ -1013,7 +1076,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="18"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10"/>
@@ -1021,7 +1084,7 @@
       <c r="E38" s="19"/>
       <c r="F38" s="20"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
@@ -1029,7 +1092,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="18"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10"/>
@@ -1037,7 +1100,7 @@
       <c r="E40" s="19"/>
       <c r="F40" s="20"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
@@ -1045,7 +1108,7 @@
       <c r="E41" s="17"/>
       <c r="F41" s="18"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="9"/>
       <c r="C42" s="10"/>
@@ -1053,7 +1116,7 @@
       <c r="E42" s="19"/>
       <c r="F42" s="20"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
@@ -1061,7 +1124,7 @@
       <c r="E43" s="17"/>
       <c r="F43" s="18"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="9"/>
       <c r="C44" s="10"/>
@@ -1069,7 +1132,7 @@
       <c r="E44" s="19"/>
       <c r="F44" s="20"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
@@ -1077,7 +1140,7 @@
       <c r="E45" s="17"/>
       <c r="F45" s="18"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10"/>
@@ -1085,7 +1148,7 @@
       <c r="E46" s="19"/>
       <c r="F46" s="20"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
@@ -1093,7 +1156,7 @@
       <c r="E47" s="17"/>
       <c r="F47" s="18"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
@@ -1101,7 +1164,7 @@
       <c r="E48" s="19"/>
       <c r="F48" s="20"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
@@ -1109,7 +1172,7 @@
       <c r="E49" s="17"/>
       <c r="F49" s="18"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
@@ -1118,16 +1181,14 @@
       <c r="F50" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1155,43 +1216,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1208,13 +1269,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
@@ -1222,7 +1283,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
@@ -1230,7 +1291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
@@ -1238,7 +1299,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
@@ -1246,17 +1307,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: Type logement "T5 et plus" => "T5" & "T6 et plus"
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CC3C32-C9B5-4672-8850-41B639590914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD57813-EF7C-4A69-A14E-C26D7B9488E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>T4</t>
-  </si>
-  <si>
-    <t>T5 et plus</t>
   </si>
   <si>
     <t>Désignation des logements</t>
@@ -139,6 +136,12 @@
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
     </r>
+  </si>
+  <si>
+    <t>T6 et plus</t>
+  </si>
+  <si>
+    <t>T5</t>
   </si>
 </sst>
 </file>
@@ -213,20 +216,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -361,42 +355,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -405,19 +401,16 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -737,7 +730,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -747,438 +740,438 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="30" t="s">
+      <c r="D1" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="159" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="159" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="32" t="s">
+      <c r="C2" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="21"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="20"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="22"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="21"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="20"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="18"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="20"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="20"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="18"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="17"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="19"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="18"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="20"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="18"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="20"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="19"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="18"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="17"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="20"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="18"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="20"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="18"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="17"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="20"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="19"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="18"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="17"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="20"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="19"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="18"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="17"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="20"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="19"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="18"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="17"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="20"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="19"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="18"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="17"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="24"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1191,18 +1184,24 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCD227EF-B54F-034B-A20F-2ABFE6AC8AED}">
           <x14:formula1>
             <xm:f>Data!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C50</xm:sqref>
+          <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{591959C4-D322-A34E-A688-5466D50E7029}">
           <x14:formula1>
             <xm:f>Data!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A50</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA715F17-5A33-4A5F-A659-F899F3721838}">
+          <x14:formula1>
+            <xm:f>Data!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:C50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1234,7 +1233,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -1249,7 +1248,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
@@ -1267,7 +1266,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1276,52 +1277,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>12</v>
+      <c r="C1" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>10</v>
+      <c r="A6" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bEDsmZ+FmACxfQF3cyUOSJYoXOIBznWdnbSx58q83o6nuQPdrWaTLPZmrKMmJTYHKXKDIN6rWdwcpkydvTos3g==" saltValue="rbBlCCMuso1zkkmD54Zvwg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jd9oczu5LHxPxedw9GHMTxgnDAiMG4CeITm668UMoGahw9qMfrufLRn64f2Vkvj6/b0RaOaPLroMmQV3loTp1w==" saltValue="C/9sYsBZKi2LSuaZhj19Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update: Type logement "T5 et plus" => "T5" & "T6 et plus" (#402)
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CC3C32-C9B5-4672-8850-41B639590914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD57813-EF7C-4A69-A14E-C26D7B9488E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>T4</t>
-  </si>
-  <si>
-    <t>T5 et plus</t>
   </si>
   <si>
     <t>Désignation des logements</t>
@@ -139,6 +136,12 @@
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
     </r>
+  </si>
+  <si>
+    <t>T6 et plus</t>
+  </si>
+  <si>
+    <t>T5</t>
   </si>
 </sst>
 </file>
@@ -213,20 +216,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -361,42 +355,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -405,19 +401,16 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -737,7 +730,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -747,438 +740,438 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="30" t="s">
+      <c r="D1" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="159" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="159" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="32" t="s">
+      <c r="C2" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="21"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="20"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="22"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="21"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="20"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="18"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="20"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="20"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="18"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="17"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="19"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="18"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="20"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="18"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="20"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="19"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="18"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="17"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="20"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="18"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="20"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="18"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="17"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="20"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="19"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="18"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="17"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="20"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="19"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="18"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="17"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="20"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="19"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="18"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="17"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="20"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="19"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="18"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="17"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="24"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1191,18 +1184,24 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCD227EF-B54F-034B-A20F-2ABFE6AC8AED}">
           <x14:formula1>
             <xm:f>Data!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C50</xm:sqref>
+          <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{591959C4-D322-A34E-A688-5466D50E7029}">
           <x14:formula1>
             <xm:f>Data!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A50</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA715F17-5A33-4A5F-A659-F899F3721838}">
+          <x14:formula1>
+            <xm:f>Data!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:C50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1234,7 +1233,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -1249,7 +1248,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
@@ -1267,7 +1266,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1276,52 +1277,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>12</v>
+      <c r="C1" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>10</v>
+      <c r="A6" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bEDsmZ+FmACxfQF3cyUOSJYoXOIBznWdnbSx58q83o6nuQPdrWaTLPZmrKMmJTYHKXKDIN6rWdwcpkydvTos3g==" saltValue="rbBlCCMuso1zkkmD54Zvwg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jd9oczu5LHxPxedw9GHMTxgnDAiMG4CeITm668UMoGahw9qMfrufLRn64f2Vkvj6/b0RaOaPLroMmQV3loTp1w==" saltValue="C/9sYsBZKi2LSuaZhj19Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update: add T1bis in files
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD57813-EF7C-4A69-A14E-C26D7B9488E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB13426-739A-4C07-8E18-5017FDB4AA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>T5</t>
+  </si>
+  <si>
+    <t>T1bis</t>
   </si>
 </sst>
 </file>
@@ -730,7 +733,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -759,7 +762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="159" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>23</v>
       </c>
@@ -1184,13 +1187,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCD227EF-B54F-034B-A20F-2ABFE6AC8AED}">
-          <x14:formula1>
-            <xm:f>Data!$A$2:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{591959C4-D322-A34E-A688-5466D50E7029}">
           <x14:formula1>
             <xm:f>Data!$C$2:$C$4</xm:f>
@@ -1199,9 +1196,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA715F17-5A33-4A5F-A659-F899F3721838}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$7</xm:f>
+            <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C50</xm:sqref>
+          <xm:sqref>C3:C50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1264,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1291,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>16</v>
@@ -1302,7 +1299,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>15</v>
@@ -1310,21 +1307,26 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jd9oczu5LHxPxedw9GHMTxgnDAiMG4CeITm668UMoGahw9qMfrufLRn64f2Vkvj6/b0RaOaPLroMmQV3loTp1w==" saltValue="C/9sYsBZKi2LSuaZhj19Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="f2+ETFU1nnGwoBW57keribWXS3yVCrYpleshJvuA2DFqLz2ovVHKnxmdRCvGKybjPXDVIEAza/xFIy6mYZxAFw==" saltValue="mNnTGPv7tdzXrR9NTdmDgg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
S666 bug type logements - ajout des T1bis (#414)
* update: Type logement "T5 et plus" => "T5" & "T6 et plus"

* update: add T1bis in files
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD57813-EF7C-4A69-A14E-C26D7B9488E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB13426-739A-4C07-8E18-5017FDB4AA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>T5</t>
+  </si>
+  <si>
+    <t>T1bis</t>
   </si>
 </sst>
 </file>
@@ -730,7 +733,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -759,7 +762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="159" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>23</v>
       </c>
@@ -1184,13 +1187,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCD227EF-B54F-034B-A20F-2ABFE6AC8AED}">
-          <x14:formula1>
-            <xm:f>Data!$A$2:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{591959C4-D322-A34E-A688-5466D50E7029}">
           <x14:formula1>
             <xm:f>Data!$C$2:$C$4</xm:f>
@@ -1199,9 +1196,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA715F17-5A33-4A5F-A659-F899F3721838}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$7</xm:f>
+            <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C50</xm:sqref>
+          <xm:sqref>C3:C50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1264,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1291,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>16</v>
@@ -1302,7 +1299,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>15</v>
@@ -1310,21 +1307,26 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jd9oczu5LHxPxedw9GHMTxgnDAiMG4CeITm668UMoGahw9qMfrufLRn64f2Vkvj6/b0RaOaPLroMmQV3loTp1w==" saltValue="C/9sYsBZKi2LSuaZhj19Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="f2+ETFU1nnGwoBW57keribWXS3yVCrYpleshJvuA2DFqLz2ovVHKnxmdRCvGKybjPXDVIEAza/xFIy6mYZxAFw==" saltValue="mNnTGPv7tdzXrR9NTdmDgg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update: annexe type (cave in cours)
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB13426-739A-4C07-8E18-5017FDB4AA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD221E1-F946-44AA-999A-0AF07DFF98FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Loyer unitaire en €</t>
-  </si>
-  <si>
-    <t>Cave</t>
   </si>
   <si>
     <t>Terrasse</t>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>T1bis</t>
+  </si>
+  <si>
+    <t>Cours</t>
   </si>
 </sst>
 </file>
@@ -358,34 +358,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -743,438 +742,438 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="31" t="s">
+      <c r="C2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="20"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="19"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="21"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="20"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="17"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="19"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="17"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="19"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="19"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="17"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="19"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="17"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="19"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="17"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="19"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="17"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="19"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="18"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="17"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="16"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="19"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="18"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="16"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="19"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="18"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="17"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="16"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="19"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="17"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="16"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="18"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="17"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="16"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="19"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="18"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="17"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="16"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="23"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1230,7 +1229,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -1245,7 +1244,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1263,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1274,59 +1273,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>25</v>
+      <c r="A7" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>24</v>
+      <c r="A8" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="f2+ETFU1nnGwoBW57keribWXS3yVCrYpleshJvuA2DFqLz2ovVHKnxmdRCvGKybjPXDVIEAza/xFIy6mYZxAFw==" saltValue="mNnTGPv7tdzXrR9NTdmDgg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="BSF21Fy593qS9aGSXO+kUGzL0t8etOGr13Ga1s7hhqkfRo2YTCNpDH15GBaaRFnGrWx0rKLvsVs8Tx1ZAA6uTA==" saltValue="/IYTcYxKW6Mpz5WVWOQOew==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
S735 replace cave by cours (#477)
* update: annexe type (cave in cours)

* update: migration & correction of cour

* update: fix coquille

* fix: tests

* fix coquille
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB13426-739A-4C07-8E18-5017FDB4AA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8DC2C2-8CAA-495B-BB15-99940904A26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11835" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Loyer unitaire en €</t>
-  </si>
-  <si>
-    <t>Cave</t>
   </si>
   <si>
     <t>Terrasse</t>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>T1bis</t>
+  </si>
+  <si>
+    <t>Cour</t>
   </si>
 </sst>
 </file>
@@ -358,34 +358,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -733,7 +732,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -743,438 +742,438 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="31" t="s">
+      <c r="C2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="20"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="19"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="21"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="20"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="17"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="19"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="17"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="19"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="19"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="17"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="19"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="17"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="19"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="17"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="19"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="17"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="19"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="18"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="17"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="16"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="19"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="18"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="16"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="19"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="18"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="17"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="16"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="19"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="17"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="16"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="18"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="17"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="16"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="19"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="18"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="17"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="16"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="23"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1230,7 +1229,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -1245,7 +1244,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1263,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1274,59 +1273,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>25</v>
+      <c r="A7" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>24</v>
+      <c r="A8" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="f2+ETFU1nnGwoBW57keribWXS3yVCrYpleshJvuA2DFqLz2ovVHKnxmdRCvGKybjPXDVIEAza/xFIy6mYZxAFw==" saltValue="mNnTGPv7tdzXrR9NTdmDgg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ymttLS9eF6ObcWJe7HqkH+T6svVP3I5bmmwFsZFhwdAXsGeXNHVEuYdifPOlcV5R5LuhSal6l7W8ZNStwxE5PQ==" saltValue="Fqzx6C7o3jXBfhc82hc8UA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix annexe label caves by cours in XLSX
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pitou/Pro/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8DC2C2-8CAA-495B-BB15-99940904A26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1117842-AFC1-4246-8ECC-D2FFAD4B5804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11835" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1040" yWindow="880" windowWidth="34960" windowHeight="22500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
@@ -104,6 +104,18 @@
     <t>(Choisir dans la liste déroulante)</t>
   </si>
   <si>
+    <t>T6 et plus</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T1bis</t>
+  </si>
+  <si>
+    <t>Cour</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">
  </t>
@@ -129,22 +141,10 @@
         <scheme val="minor"/>
       </rPr>
       <t>(Choisir dans la liste déroulante. 
-Les annexes concernées sont ici les jardins, les caves et les surfaces de terrasse au-delà de 9 m²
+Les annexes concernées sont ici les jardins, les cours et les surfaces de terrasse au-delà de 9 m²
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
     </r>
-  </si>
-  <si>
-    <t>T6 et plus</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T1bis</t>
-  </si>
-  <si>
-    <t>Cour</t>
   </si>
 </sst>
 </file>
@@ -732,16 +732,16 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.75" customWidth="1"/>
-    <col min="2" max="6" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="6" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -761,9 +761,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>20</v>
@@ -775,7 +775,7 @@
       <c r="E2" s="35"/>
       <c r="F2" s="33"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -783,7 +783,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -791,7 +791,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -807,7 +807,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -823,7 +823,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -831,7 +831,7 @@
       <c r="E7" s="15"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -839,7 +839,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
@@ -847,7 +847,7 @@
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -855,7 +855,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
@@ -863,7 +863,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -871,7 +871,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -879,7 +879,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="16"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -887,7 +887,7 @@
       <c r="E14" s="17"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -895,7 +895,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -903,7 +903,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -911,7 +911,7 @@
       <c r="E17" s="15"/>
       <c r="F17" s="16"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -919,7 +919,7 @@
       <c r="E18" s="17"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -927,7 +927,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -935,7 +935,7 @@
       <c r="E20" s="17"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
@@ -943,7 +943,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -951,7 +951,7 @@
       <c r="E22" s="17"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
@@ -959,7 +959,7 @@
       <c r="E23" s="15"/>
       <c r="F23" s="16"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -967,7 +967,7 @@
       <c r="E24" s="17"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
@@ -975,7 +975,7 @@
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -983,7 +983,7 @@
       <c r="E26" s="17"/>
       <c r="F26" s="18"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
@@ -991,7 +991,7 @@
       <c r="E27" s="15"/>
       <c r="F27" s="16"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -999,7 +999,7 @@
       <c r="E28" s="17"/>
       <c r="F28" s="18"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
@@ -1007,7 +1007,7 @@
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
@@ -1015,7 +1015,7 @@
       <c r="E30" s="17"/>
       <c r="F30" s="18"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
@@ -1023,7 +1023,7 @@
       <c r="E31" s="15"/>
       <c r="F31" s="16"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -1031,7 +1031,7 @@
       <c r="E32" s="17"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -1039,7 +1039,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="16"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
@@ -1047,7 +1047,7 @@
       <c r="E34" s="17"/>
       <c r="F34" s="18"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
@@ -1055,7 +1055,7 @@
       <c r="E35" s="15"/>
       <c r="F35" s="16"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
@@ -1063,7 +1063,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="18"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
@@ -1071,7 +1071,7 @@
       <c r="E37" s="15"/>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
@@ -1079,7 +1079,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="18"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
@@ -1087,7 +1087,7 @@
       <c r="E39" s="15"/>
       <c r="F39" s="16"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
@@ -1095,7 +1095,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="18"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
@@ -1103,7 +1103,7 @@
       <c r="E41" s="15"/>
       <c r="F41" s="16"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
@@ -1111,7 +1111,7 @@
       <c r="E42" s="17"/>
       <c r="F42" s="18"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
@@ -1119,7 +1119,7 @@
       <c r="E43" s="15"/>
       <c r="F43" s="16"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
@@ -1127,7 +1127,7 @@
       <c r="E44" s="17"/>
       <c r="F44" s="18"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
@@ -1135,7 +1135,7 @@
       <c r="E45" s="15"/>
       <c r="F45" s="16"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
@@ -1143,7 +1143,7 @@
       <c r="E46" s="17"/>
       <c r="F46" s="18"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
@@ -1151,7 +1151,7 @@
       <c r="E47" s="15"/>
       <c r="F47" s="16"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
@@ -1159,7 +1159,7 @@
       <c r="E48" s="17"/>
       <c r="F48" s="18"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -1167,7 +1167,7 @@
       <c r="E49" s="15"/>
       <c r="F49" s="16"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
@@ -1211,43 +1211,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1266,13 +1266,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
@@ -1280,23 +1280,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
@@ -1304,24 +1304,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Petites améliorations: bouton de support & label annexe Excel (#740)
* Disable mailto corner chip if in SIAP context

* Fix annexe label caves by cours in XLSX
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pitou/Pro/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8DC2C2-8CAA-495B-BB15-99940904A26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1117842-AFC1-4246-8ECC-D2FFAD4B5804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11835" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1040" yWindow="880" windowWidth="34960" windowHeight="22500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
@@ -104,6 +104,18 @@
     <t>(Choisir dans la liste déroulante)</t>
   </si>
   <si>
+    <t>T6 et plus</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T1bis</t>
+  </si>
+  <si>
+    <t>Cour</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">
  </t>
@@ -129,22 +141,10 @@
         <scheme val="minor"/>
       </rPr>
       <t>(Choisir dans la liste déroulante. 
-Les annexes concernées sont ici les jardins, les caves et les surfaces de terrasse au-delà de 9 m²
+Les annexes concernées sont ici les jardins, les cours et les surfaces de terrasse au-delà de 9 m²
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
     </r>
-  </si>
-  <si>
-    <t>T6 et plus</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T1bis</t>
-  </si>
-  <si>
-    <t>Cour</t>
   </si>
 </sst>
 </file>
@@ -732,16 +732,16 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.75" customWidth="1"/>
-    <col min="2" max="6" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="6" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -761,9 +761,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>20</v>
@@ -775,7 +775,7 @@
       <c r="E2" s="35"/>
       <c r="F2" s="33"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -783,7 +783,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -791,7 +791,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -807,7 +807,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -823,7 +823,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -831,7 +831,7 @@
       <c r="E7" s="15"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -839,7 +839,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
@@ -847,7 +847,7 @@
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -855,7 +855,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
@@ -863,7 +863,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -871,7 +871,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -879,7 +879,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="16"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -887,7 +887,7 @@
       <c r="E14" s="17"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -895,7 +895,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -903,7 +903,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -911,7 +911,7 @@
       <c r="E17" s="15"/>
       <c r="F17" s="16"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -919,7 +919,7 @@
       <c r="E18" s="17"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -927,7 +927,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -935,7 +935,7 @@
       <c r="E20" s="17"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
@@ -943,7 +943,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -951,7 +951,7 @@
       <c r="E22" s="17"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
@@ -959,7 +959,7 @@
       <c r="E23" s="15"/>
       <c r="F23" s="16"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -967,7 +967,7 @@
       <c r="E24" s="17"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
@@ -975,7 +975,7 @@
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -983,7 +983,7 @@
       <c r="E26" s="17"/>
       <c r="F26" s="18"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
@@ -991,7 +991,7 @@
       <c r="E27" s="15"/>
       <c r="F27" s="16"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -999,7 +999,7 @@
       <c r="E28" s="17"/>
       <c r="F28" s="18"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
@@ -1007,7 +1007,7 @@
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
@@ -1015,7 +1015,7 @@
       <c r="E30" s="17"/>
       <c r="F30" s="18"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
@@ -1023,7 +1023,7 @@
       <c r="E31" s="15"/>
       <c r="F31" s="16"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -1031,7 +1031,7 @@
       <c r="E32" s="17"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -1039,7 +1039,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="16"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
@@ -1047,7 +1047,7 @@
       <c r="E34" s="17"/>
       <c r="F34" s="18"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
@@ -1055,7 +1055,7 @@
       <c r="E35" s="15"/>
       <c r="F35" s="16"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
@@ -1063,7 +1063,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="18"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
@@ -1071,7 +1071,7 @@
       <c r="E37" s="15"/>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
@@ -1079,7 +1079,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="18"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
@@ -1087,7 +1087,7 @@
       <c r="E39" s="15"/>
       <c r="F39" s="16"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
@@ -1095,7 +1095,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="18"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
@@ -1103,7 +1103,7 @@
       <c r="E41" s="15"/>
       <c r="F41" s="16"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
@@ -1111,7 +1111,7 @@
       <c r="E42" s="17"/>
       <c r="F42" s="18"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
@@ -1119,7 +1119,7 @@
       <c r="E43" s="15"/>
       <c r="F43" s="16"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
@@ -1127,7 +1127,7 @@
       <c r="E44" s="17"/>
       <c r="F44" s="18"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
@@ -1135,7 +1135,7 @@
       <c r="E45" s="15"/>
       <c r="F45" s="16"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
@@ -1143,7 +1143,7 @@
       <c r="E46" s="17"/>
       <c r="F46" s="18"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
@@ -1151,7 +1151,7 @@
       <c r="E47" s="15"/>
       <c r="F47" s="16"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
@@ -1159,7 +1159,7 @@
       <c r="E48" s="17"/>
       <c r="F48" s="18"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -1167,7 +1167,7 @@
       <c r="E49" s="15"/>
       <c r="F49" s="16"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
@@ -1211,43 +1211,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1266,13 +1266,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
@@ -1280,23 +1280,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
@@ -1304,24 +1304,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revue des styles des xlsx
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pitou/Pro/apilos/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1117842-AFC1-4246-8ECC-D2FFAD4B5804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20D8BCC-D0A9-3A4A-A2F3-6A66B77D81DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="880" windowWidth="34960" windowHeight="22500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="34840" yWindow="1280" windowWidth="28880" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
     <sheet name="Notice" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -219,49 +219,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -358,61 +321,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -433,9 +389,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -473,7 +429,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -579,7 +535,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -721,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -729,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
-  <dimension ref="A1:O50"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,62 +698,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="23"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:15" ht="20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="23"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="19"/>
+      <c r="F5" s="16"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -807,373 +771,357 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="20"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="23"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="15"/>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="23"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="23"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="23"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="15"/>
       <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="23"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="15"/>
       <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="23"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="15"/>
       <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="23"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="15"/>
       <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="23"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="23"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="15"/>
       <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="23"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="23"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="15"/>
       <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="18"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
-      <c r="D29" s="23"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="23"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="15"/>
       <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="18"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="23"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="15"/>
       <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="18"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="23"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="15"/>
       <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="18"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="23"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="15"/>
       <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="18"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="23"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="15"/>
       <c r="F39" s="16"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="18"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="23"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="15"/>
       <c r="F41" s="16"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="18"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
-      <c r="D43" s="23"/>
+      <c r="D43" s="18"/>
       <c r="E43" s="15"/>
       <c r="F43" s="16"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="18"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
-      <c r="D45" s="23"/>
+      <c r="D45" s="18"/>
       <c r="E45" s="15"/>
       <c r="F45" s="16"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="18"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
-      <c r="D47" s="23"/>
+      <c r="D47" s="18"/>
       <c r="E47" s="15"/>
       <c r="F47" s="16"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="18"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="23"/>
+      <c r="D49" s="18"/>
       <c r="E49" s="15"/>
       <c r="F49" s="16"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1191,13 +1139,13 @@
           <x14:formula1>
             <xm:f>Data!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A50</xm:sqref>
+          <xm:sqref>A3:A49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA715F17-5A33-4A5F-A659-F899F3721838}">
           <x14:formula1>
             <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C50</xm:sqref>
+          <xm:sqref>C3:C49</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1262,9 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1273,54 +1219,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
revue des styles des xlsx (#1725)
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pitou/Pro/apilos/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1117842-AFC1-4246-8ECC-D2FFAD4B5804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20D8BCC-D0A9-3A4A-A2F3-6A66B77D81DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="880" windowWidth="34960" windowHeight="22500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="34840" yWindow="1280" windowWidth="28880" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
     <sheet name="Notice" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -219,49 +219,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -358,61 +321,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -433,9 +389,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -473,7 +429,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -579,7 +535,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -721,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -729,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
-  <dimension ref="A1:O50"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,62 +698,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="23"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:15" ht="20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="23"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="19"/>
+      <c r="F5" s="16"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -807,373 +771,357 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="20"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="23"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="15"/>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="23"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="23"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="23"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="15"/>
       <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="23"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="15"/>
       <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="23"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="15"/>
       <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="23"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="15"/>
       <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="23"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="23"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="15"/>
       <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="23"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="23"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="15"/>
       <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="18"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
-      <c r="D29" s="23"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="23"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="15"/>
       <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="18"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="23"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="15"/>
       <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="18"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="23"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="15"/>
       <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="18"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="23"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="15"/>
       <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="18"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="23"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="15"/>
       <c r="F39" s="16"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="18"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="23"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="15"/>
       <c r="F41" s="16"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="18"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
-      <c r="D43" s="23"/>
+      <c r="D43" s="18"/>
       <c r="E43" s="15"/>
       <c r="F43" s="16"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="18"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
-      <c r="D45" s="23"/>
+      <c r="D45" s="18"/>
       <c r="E45" s="15"/>
       <c r="F45" s="16"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="18"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
-      <c r="D47" s="23"/>
+      <c r="D47" s="18"/>
       <c r="E47" s="15"/>
       <c r="F47" s="16"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="18"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="23"/>
+      <c r="D49" s="18"/>
       <c r="E49" s="15"/>
       <c r="F49" s="16"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1191,13 +1139,13 @@
           <x14:formula1>
             <xm:f>Data!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A50</xm:sqref>
+          <xm:sqref>A3:A49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA715F17-5A33-4A5F-A659-F899F3721838}">
           <x14:formula1>
             <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C50</xm:sqref>
+          <xm:sqref>C3:C49</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1262,9 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1273,54 +1219,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: include mixte conventions
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayoub.bouchachia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20D8BCC-D0A9-3A4A-A2F3-6A66B77D81DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D331DA-C53B-4D0D-88AB-B2FE2949555A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34840" yWindow="1280" windowWidth="28880" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -145,6 +145,9 @@
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
     </r>
+  </si>
+  <si>
+    <t>Financement</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -688,434 +691,478 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" customWidth="1"/>
-    <col min="2" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="44.625" customWidth="1"/>
+    <col min="2" max="6" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F2" s="28"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="18"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C6" s="17"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C7" s="18"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C8" s="17"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C9" s="18"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C10" s="17"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C11" s="18"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C12" s="17"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C13" s="18"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C14" s="17"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C15" s="18"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="17"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="18"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="17"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="18"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="17"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="18"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="17"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="18"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="17"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="18"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="17"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="18"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="17"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C29" s="18"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="17"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="16"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="18"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="17"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="18"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="14"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C34" s="17"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="16"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="18"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="17"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="16"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="18"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="17"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="16"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C39" s="18"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="16"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C40" s="17"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C41" s="18"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="16"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="14"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C42" s="17"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="16"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C43" s="18"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="16"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="14"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C44" s="17"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C45" s="18"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="16"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="14"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C46" s="17"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="16"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C47" s="18"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="16"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C48" s="17"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -1124,10 +1171,11 @@
       <c r="F49" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1145,7 +1193,7 @@
           <x14:formula1>
             <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C49</xm:sqref>
+          <xm:sqref>C49 D3:D48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1159,43 +1207,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1212,13 +1260,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
@@ -1242,7 +1290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -1250,22 +1298,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Avenant for convention mixte latest (#2038)
---------
Co-authored-by: Ayoub BOUCHACHIA <ayoub.bouchachia@sully-group.com>
Co-authored-by: adrien.abescat <adrien.abescat@sullly-group.fr>
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayoub.bouchachia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20D8BCC-D0A9-3A4A-A2F3-6A66B77D81DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D331DA-C53B-4D0D-88AB-B2FE2949555A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34840" yWindow="1280" windowWidth="28880" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -145,6 +145,9 @@
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
     </r>
+  </si>
+  <si>
+    <t>Financement</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -688,434 +691,478 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" customWidth="1"/>
-    <col min="2" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="44.625" customWidth="1"/>
+    <col min="2" max="6" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F2" s="28"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="18"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C6" s="17"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C7" s="18"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C8" s="17"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C9" s="18"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C10" s="17"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C11" s="18"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C12" s="17"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C13" s="18"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C14" s="17"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C15" s="18"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="17"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="18"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="17"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="18"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="17"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="18"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="17"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="18"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="17"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="18"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="17"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="18"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="17"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C29" s="18"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="17"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="16"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="18"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="17"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="18"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="14"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C34" s="17"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="16"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="18"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="17"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="16"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="18"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="17"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="16"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C39" s="18"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="16"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C40" s="17"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C41" s="18"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="16"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="14"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C42" s="17"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="16"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C43" s="18"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="16"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="14"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C44" s="17"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C45" s="18"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="16"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="14"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C46" s="17"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="16"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C47" s="18"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="16"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C48" s="17"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -1124,10 +1171,11 @@
       <c r="F49" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1145,7 +1193,7 @@
           <x14:formula1>
             <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C49</xm:sqref>
+          <xm:sqref>C49 D3:D48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1159,43 +1207,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1212,13 +1260,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
@@ -1242,7 +1290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -1250,22 +1298,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Revert "Avenant for convention mixte latest (#2038)"
This reverts commit bf33b464bd89d690600d8c0de2fba5598789307b.
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayoub.bouchachia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D331DA-C53B-4D0D-88AB-B2FE2949555A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20D8BCC-D0A9-3A4A-A2F3-6A66B77D81DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="34840" yWindow="1280" windowWidth="28880" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -145,9 +145,6 @@
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
     </r>
-  </si>
-  <si>
-    <t>Financement</t>
   </si>
 </sst>
 </file>
@@ -392,7 +389,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -691,478 +688,434 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.625" customWidth="1"/>
-    <col min="2" max="6" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="6" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="21" t="s">
         <v>12</v>
       </c>
+      <c r="D1" s="27" t="s">
+        <v>16</v>
+      </c>
       <c r="E1" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="24" t="s">
+      <c r="C2" s="24" t="s">
         <v>21</v>
       </c>
+      <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="6"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="6"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="4"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="6"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="4"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="6"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="4"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="6"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="6"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="4"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="6"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="6"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="6"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="4"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="6"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="6"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="4"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="6"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="4"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="6"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="4"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="6"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="6"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="4"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="6"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="4"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="16"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="6"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="16"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="4"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="16"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="6"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="16"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="4"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="16"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="6"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="16"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="14"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="4"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="14"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="16"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="6"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="16"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="14"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="4"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="14"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="16"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="6"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="16"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="14"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="4"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -1171,11 +1124,10 @@
       <c r="F49" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="G1:G2"/>
+  <mergeCells count="3">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1193,7 +1145,7 @@
           <x14:formula1>
             <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C49 D3:D48</xm:sqref>
+          <xm:sqref>C3:C49</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1207,43 +1159,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1260,13 +1212,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -1274,7 +1226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
@@ -1290,7 +1242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -1298,22 +1250,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Revert "Avenant for convention mixte latest (#2038)" (#2063)
This reverts commit bf33b464bd89d690600d8c0de2fba5598789307b.
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayoub.bouchachia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D331DA-C53B-4D0D-88AB-B2FE2949555A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20D8BCC-D0A9-3A4A-A2F3-6A66B77D81DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="34840" yWindow="1280" windowWidth="28880" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -145,9 +145,6 @@
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
     </r>
-  </si>
-  <si>
-    <t>Financement</t>
   </si>
 </sst>
 </file>
@@ -392,7 +389,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -691,478 +688,434 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.625" customWidth="1"/>
-    <col min="2" max="6" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="6" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="21" t="s">
         <v>12</v>
       </c>
+      <c r="D1" s="27" t="s">
+        <v>16</v>
+      </c>
       <c r="E1" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="24" t="s">
+      <c r="C2" s="24" t="s">
         <v>21</v>
       </c>
+      <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="6"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="6"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="4"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="6"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="4"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="6"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="4"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="6"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="6"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="4"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="6"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="6"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="6"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="4"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="6"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="6"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="4"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="6"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="4"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="6"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="4"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="6"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="6"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="4"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="6"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="4"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="16"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="6"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="16"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="4"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="16"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="6"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="16"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="4"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="16"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="6"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="16"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="14"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="4"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="14"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="16"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="6"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="16"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="14"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="4"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="14"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="16"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="6"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="16"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="14"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="4"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -1171,11 +1124,10 @@
       <c r="F49" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="G1:G2"/>
+  <mergeCells count="3">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1193,7 +1145,7 @@
           <x14:formula1>
             <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C49 D3:D48</xm:sqref>
+          <xm:sqref>C3:C49</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1207,43 +1159,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1260,13 +1212,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -1274,7 +1226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
@@ -1290,7 +1242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -1298,22 +1250,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Avenant for convention mixte latest to recette (#2064)
* feat: include mixte conventions

* mise à jour des templates de generation des conventions mixtes (#2062)


---------

Co-authored-by: Ayoub BOUCHACHIA <ayoub.bouchachia@sully-group.com>
Co-authored-by: adrien.abescat <adrien.abescat@sullly-group.fr>
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayoub.bouchachia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20D8BCC-D0A9-3A4A-A2F3-6A66B77D81DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D331DA-C53B-4D0D-88AB-B2FE2949555A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34840" yWindow="1280" windowWidth="28880" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Annexes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -145,6 +145,9 @@
 ( ex : Pour une terrasse d’une surface totale de 10 m², renseignez ici uniquement 1 m², les 9m² sont intégrés dans le calcul de la surface utile).
 La déclaration des stationnements par type se fera à la prochaine étape)</t>
     </r>
+  </si>
+  <si>
+    <t>Financement</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -688,434 +691,478 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" customWidth="1"/>
-    <col min="2" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="44.625" customWidth="1"/>
+    <col min="2" max="6" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F2" s="28"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="18"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C6" s="17"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C7" s="18"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C8" s="17"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C9" s="18"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C10" s="17"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C11" s="18"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C12" s="17"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C13" s="18"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C14" s="17"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C15" s="18"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="17"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="18"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="17"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="18"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="17"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="18"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="17"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="18"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="17"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="18"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="17"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="18"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="17"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C29" s="18"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="17"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="16"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="18"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="17"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="18"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="14"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C34" s="17"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="16"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="18"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="17"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="16"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="18"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="17"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="16"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C39" s="18"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="16"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C40" s="17"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C41" s="18"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="16"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="14"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C42" s="17"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="16"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C43" s="18"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="16"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="14"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C44" s="17"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C45" s="18"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="16"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="14"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C46" s="17"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="16"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C47" s="18"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="16"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C48" s="17"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -1124,10 +1171,11 @@
       <c r="F49" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1145,7 +1193,7 @@
           <x14:formula1>
             <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C49</xm:sqref>
+          <xm:sqref>C49 D3:D48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1159,43 +1207,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1212,13 +1260,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
@@ -1242,7 +1290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -1250,22 +1298,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>22</v>
       </c>

</xml_diff>